<commit_message>
add general information data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/IR.xlsx
+++ b/src/test/resources/testdata/IR.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldu\git\d3securityautomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D782BA-98D1-4425-876A-C6C1CE3A3CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703EB139-A555-484C-AC9E-1EBA793DC99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="3360" windowWidth="32940" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="IR_General information" sheetId="1" r:id="rId1"/>
+    <sheet name="testIR_GeneralInformation" sheetId="1" r:id="rId1"/>
     <sheet name="IR_Tasks" sheetId="2" r:id="rId2"/>
     <sheet name="IR_Location" sheetId="3" r:id="rId3"/>
     <sheet name="IR_TrackingLog" sheetId="4" r:id="rId4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>CaseID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>IncidentEndedOn</t>
   </si>
   <si>
-    <t>SemdOneTimeEmailNotificationOnSave</t>
-  </si>
-  <si>
     <t>Notifications</t>
   </si>
   <si>
@@ -105,19 +102,37 @@
     <t xml:space="preserve">UseEmailNotificationAssignmentRules </t>
   </si>
   <si>
-    <t>NotifyCCRecipientsonCreateEditandClose</t>
-  </si>
-  <si>
-    <t>OnIRCreateandEdit</t>
-  </si>
-  <si>
-    <t>OnIRClose</t>
-  </si>
-  <si>
-    <t>OnAssigneeReassign</t>
-  </si>
-  <si>
     <t>This is for testing section: General information</t>
+  </si>
+  <si>
+    <t>SendOneTimeEmailNotificationOnSave</t>
+  </si>
+  <si>
+    <t>NotifyCCRecipientsOnCreateEditandClose</t>
+  </si>
+  <si>
+    <t>Creator_OnIRCreateandEdit</t>
+  </si>
+  <si>
+    <t>Creator_OnIRClose</t>
+  </si>
+  <si>
+    <t>Creator_OnAssigneeReassign</t>
+  </si>
+  <si>
+    <t>Assignee_OnIRCreateandEdit</t>
+  </si>
+  <si>
+    <t>Assignee_OnIRClose</t>
+  </si>
+  <si>
+    <t>Assignee_OnAssigneeReassign</t>
+  </si>
+  <si>
+    <t>DropDownOption</t>
+  </si>
+  <si>
+    <t>Incident Report</t>
   </si>
 </sst>
 </file>
@@ -453,7 +468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -461,24 +478,26 @@
     <col min="2" max="2" width="32.140625" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="10" width="16.5703125" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="15" width="50" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" customWidth="1"/>
-    <col min="18" max="18" width="27.7109375" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="22" width="13.28515625" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" customWidth="1"/>
-    <col min="24" max="24" width="19.7109375" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="11" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" customWidth="1"/>
+    <col min="16" max="16" width="50" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="18" max="18" width="24.85546875" customWidth="1"/>
+    <col min="19" max="19" width="27.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.7109375" customWidth="1"/>
+    <col min="22" max="23" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="28.85546875" customWidth="1"/>
+    <col min="25" max="25" width="36.85546875" customWidth="1"/>
+    <col min="26" max="26" width="27.28515625" customWidth="1"/>
+    <col min="27" max="27" width="43.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -495,52 +514,52 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>27</v>
@@ -549,25 +568,27 @@
         <v>28</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA1" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -576,34 +597,37 @@
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="2" t="b">
+      <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="2" t="b">
+      <c r="L2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" t="b">
+      <c r="P2" t="b">
         <v>0</v>
       </c>
-      <c r="P2" t="b">
+      <c r="Q2" t="b">
         <v>1</v>
       </c>
-      <c r="S2" t="b">
+      <c r="T2" t="b">
         <v>1</v>
       </c>
-      <c r="W2" t="b">
+      <c r="X2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add IR generalinformation test script
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/IR.xlsx
+++ b/src/test/resources/testdata/IR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldu\git\d3securityautomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703EB139-A555-484C-AC9E-1EBA793DC99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C740CDC0-3E9D-4073-AC4E-63BB33C7F6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="3360" windowWidth="32940" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testIR_GeneralInformation" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>CaseID</t>
   </si>
@@ -133,6 +133,45 @@
   </si>
   <si>
     <t>Incident Report</t>
+  </si>
+  <si>
+    <t>ArrestDetails</t>
+  </si>
+  <si>
+    <t>WorkplaceViolence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TypeofAccident </t>
+  </si>
+  <si>
+    <t>RequiredField</t>
+  </si>
+  <si>
+    <t>MandatoryonSave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MandatoryonClose </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Posture</t>
+  </si>
+  <si>
+    <t>Hitech</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation test new Incident Report </t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -177,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -185,7 +224,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,9 +545,15 @@
     <col min="25" max="25" width="36.85546875" customWidth="1"/>
     <col min="26" max="26" width="27.28515625" customWidth="1"/>
     <col min="27" max="27" width="43.28515625" customWidth="1"/>
+    <col min="28" max="28" width="15.28515625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="17" style="2" customWidth="1"/>
+    <col min="31" max="31" width="8.85546875" style="2"/>
+    <col min="32" max="32" width="18.28515625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="19.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,53 +635,118 @@
       <c r="AA1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AB1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="b">
+      <c r="L2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1</v>
+      </c>
+      <c r="O2" s="4">
+        <v>28</v>
+      </c>
+      <c r="P2" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="X2" t="b">
-        <v>1</v>
+      <c r="Q2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="V2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add all elements data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/IR.xlsx
+++ b/src/test/resources/testdata/IR.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldu\git\d3securityautomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A1F79F-5894-4170-B11F-02D73315F690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA173D4F-9FBC-48C9-9D95-35413F8BA9AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1185" yWindow="5580" windowWidth="29010" windowHeight="9135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_IR_GeneralInformation" sheetId="1" r:id="rId1"/>
-    <sheet name="IR_Tasks" sheetId="2" r:id="rId2"/>
+    <sheet name="test_IR_AllElements" sheetId="2" r:id="rId2"/>
     <sheet name="IR_Location" sheetId="3" r:id="rId3"/>
     <sheet name="IR_TrackingLog" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
   <si>
     <t>CaseID</t>
   </si>
@@ -175,6 +175,111 @@
   </si>
   <si>
     <t>ldu@d3security.com</t>
+  </si>
+  <si>
+    <t>This is for testing section: All elements</t>
+  </si>
+  <si>
+    <t>CheckBox</t>
+  </si>
+  <si>
+    <t>DropDownMenu</t>
+  </si>
+  <si>
+    <t>list 3</t>
+  </si>
+  <si>
+    <t>ListBox</t>
+  </si>
+  <si>
+    <t>RadioBox</t>
+  </si>
+  <si>
+    <t>Radio 2</t>
+  </si>
+  <si>
+    <t>RevealCheckBox1-1</t>
+  </si>
+  <si>
+    <t>RevealCheckBox1-2</t>
+  </si>
+  <si>
+    <t>RadioBoxLevel</t>
+  </si>
+  <si>
+    <t>test 3</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>ProvinceDropdown</t>
+  </si>
+  <si>
+    <t>StateDropdown</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>CountryDropdown</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>TimeControlHour</t>
+  </si>
+  <si>
+    <t>TimeControlMin</t>
+  </si>
+  <si>
+    <t>NoonPicker</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>CalendarControl</t>
+  </si>
+  <si>
+    <t>CurrencyTextBox</t>
+  </si>
+  <si>
+    <t>CurrencyDropdown</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>SumUpAmount</t>
+  </si>
+  <si>
+    <t>SearchableTextBox</t>
+  </si>
+  <si>
+    <t>SearchableTextBoxArea</t>
+  </si>
+  <si>
+    <t>TextArea</t>
+  </si>
+  <si>
+    <t>New Incident Report - Automation Test</t>
+  </si>
+  <si>
+    <t>TextBox</t>
+  </si>
+  <si>
+    <t>Text box Input test</t>
+  </si>
+  <si>
+    <t>TextAreaReadOnly</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>Automation all elements</t>
   </si>
 </sst>
 </file>
@@ -228,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -247,6 +352,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -531,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,13 +890,219 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE9BD0B-7D82-4ECC-9256-751D07419CC2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.28515625" customWidth="1"/>
+    <col min="20" max="21" width="16" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" customWidth="1"/>
+    <col min="23" max="23" width="18.85546875" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" customWidth="1"/>
+    <col min="25" max="25" width="18.85546875" customWidth="1"/>
+    <col min="26" max="26" width="23" customWidth="1"/>
+    <col min="28" max="28" width="17" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2">
+        <v>7</v>
+      </c>
+      <c r="S2">
+        <v>55</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2">
+        <v>25</v>
+      </c>
+      <c r="V2">
+        <v>9999999</v>
+      </c>
+      <c r="W2" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>